<commit_message>
update manage user (admin)
</commit_message>
<xml_diff>
--- a/public/template_user.xlsx
+++ b/public/template_user.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PBL_SEM_5\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBB64B2-8CBD-4D7E-B48C-9B32E4BE4DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620306BA-DD19-4061-BD16-1C707A8D53BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2292" yWindow="1800" windowWidth="11256" windowHeight="9420" xr2:uid="{54818A27-3A13-4F33-B9E9-1C78F6CDF2D0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{54818A27-3A13-4F33-B9E9-1C78F6CDF2D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -63,16 +63,30 @@
   </si>
   <si>
     <t>M. Isroqi Gelby F.</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>dosen@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,13 +109,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23159750-9026-414E-B834-F59EBB09DC96}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,11 +442,11 @@
     <col min="1" max="1" width="12.21875" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -443,10 +460,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3</v>
       </c>
@@ -459,11 +479,17 @@
       <c r="D2">
         <v>1818181818</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
         <v>123456</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{8DBC90CA-8A10-4D99-A879-916C85F84EBD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>